<commit_message>
update and bug fix
</commit_message>
<xml_diff>
--- a/Data_inputs/PSERS_PlanInfo_AV2016.xlsx
+++ b/Data_inputs/PSERS_PlanInfo_AV2016.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14010" tabRatio="849" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14010" tabRatio="849" firstSheet="8" activeTab="20"/>
   </bookViews>
   <sheets>
     <sheet name="TOC" sheetId="31" r:id="rId1"/>
@@ -7412,8 +7412,8 @@
   <sheetPr codeName="Sheet15"/>
   <dimension ref="A1:D63"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I71" sqref="I71"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O35" sqref="O35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8175,7 +8175,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
@@ -9147,8 +9147,8 @@
   <sheetPr codeName="Sheet17"/>
   <dimension ref="A1:E73"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G67" sqref="G67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>